<commit_message>
Upload tree DBH and hollow data mk2
</commit_message>
<xml_diff>
--- a/datasets/tree_DBH_hollows/input/Plot 03.xlsx
+++ b/datasets/tree_DBH_hollows/input/Plot 03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickjolly/Desktop/tfn tree_hollows/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickjolly/Desktop/tfn/DataScienceProject/datasets/tree_DBH_hollows/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6C6F2E-C66F-E14A-88A8-A2B46A08FA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FE1627-D7C8-F14C-BC36-86190EC05A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="500" windowWidth="18580" windowHeight="16220" xr2:uid="{87FCBAA5-73AC-7F4D-BA18-7613AAC3B7D6}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="16220" xr2:uid="{87FCBAA5-73AC-7F4D-BA18-7613AAC3B7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="20">
   <si>
     <t>Tree Number</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>(need to complete 2 trees on 5th side plot?)</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>#255 lost tag, changed to #242</t>
@@ -462,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6190B31-262D-4A48-A546-5291A0810464}">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="86" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:B77"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N75" sqref="N75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5">
         <v>14</v>
@@ -633,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6">
         <v>16</v>
@@ -714,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9">
         <v>29</v>
@@ -1355,13 +1352,13 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D40">
         <v>45.6</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -1373,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="L40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -1384,13 +1381,13 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D41">
         <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1402,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="L41" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -1413,10 +1410,10 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -1427,13 +1424,13 @@
         <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D43">
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1445,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -1459,10 +1456,10 @@
         <v>41.9</v>
       </c>
       <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="J44" t="s">
         <v>14</v>
-      </c>
-      <c r="J44" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -1473,13 +1470,13 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D45">
         <v>45.3</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -1491,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="L45" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -1502,19 +1499,19 @@
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D46">
         <v>41.8</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L46" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -1525,13 +1522,13 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D47">
         <v>37.799999999999997</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -1543,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="L47" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -1554,13 +1551,13 @@
         <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D48">
         <v>38</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1572,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="L48" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -1583,13 +1580,13 @@
         <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D49">
         <v>39</v>
       </c>
       <c r="E49" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1601,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="L49" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -1612,13 +1609,13 @@
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D50">
         <v>38.799999999999997</v>
       </c>
       <c r="E50" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -1630,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="L50" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -1641,13 +1638,13 @@
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D51">
         <v>49.1</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -1659,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="L51" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -1670,13 +1667,13 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D52">
         <v>43</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -1688,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="L52" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -1699,13 +1696,13 @@
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D53">
         <v>48</v>
       </c>
       <c r="E53" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -1717,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="L53" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -1728,13 +1725,13 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D54">
         <v>40</v>
       </c>
       <c r="E54" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -1746,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -1757,13 +1754,13 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D55">
         <v>33</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -1775,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="L55" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -1786,13 +1783,13 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D56">
         <v>33.5</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1812,13 +1809,13 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D57">
         <v>38.1</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -1830,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -1841,7 +1838,7 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D58">
         <v>26.7</v>
@@ -1856,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="L58" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -1867,7 +1864,7 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D59">
         <v>28.5</v>
@@ -1882,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="L59" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -1893,7 +1890,7 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D60">
         <v>35.4</v>
@@ -1908,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -1919,7 +1916,7 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D61">
         <v>31.6</v>
@@ -1934,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="L61" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -1945,7 +1942,7 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D62">
         <v>35.299999999999997</v>
@@ -1960,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -1971,7 +1968,7 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D63">
         <v>24.5</v>
@@ -1986,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="L63" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -1997,7 +1994,7 @@
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D64">
         <v>32</v>
@@ -2012,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -2023,7 +2020,7 @@
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D65">
         <v>27</v>
@@ -2038,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="L65" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -2049,7 +2046,7 @@
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D66">
         <v>27.3</v>
@@ -2064,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="L66" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -2075,7 +2072,7 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D67">
         <v>23.4</v>
@@ -2090,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -2101,7 +2098,7 @@
         <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D68">
         <v>28</v>
@@ -2116,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="L68" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -2127,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D69">
         <v>29.2</v>
@@ -2142,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="L69" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
@@ -2153,7 +2150,7 @@
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D70">
         <v>34</v>
@@ -2168,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -2179,7 +2176,7 @@
         <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D71">
         <v>36.799999999999997</v>
@@ -2194,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="L71" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -2205,7 +2202,7 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D72">
         <v>37.4</v>
@@ -2220,7 +2217,7 @@
         <v>0</v>
       </c>
       <c r="L72" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
@@ -2231,7 +2228,7 @@
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D73">
         <v>33.5</v>
@@ -2246,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
@@ -2257,7 +2254,7 @@
         <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D74">
         <v>43.7</v>
@@ -2272,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="L74" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
@@ -2283,7 +2280,7 @@
         <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D75">
         <v>38.299999999999997</v>
@@ -2298,7 +2295,7 @@
         <v>0</v>
       </c>
       <c r="L75" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
@@ -2309,7 +2306,7 @@
         <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D76">
         <v>32.5</v>
@@ -2324,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="L76" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
@@ -2335,13 +2332,13 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D77">
         <v>33</v>
       </c>
       <c r="L77" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>